<commit_message>
Yourn shit is ready
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owenr\Documents\github\transboundary_fisheries_status\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renatomolina/Box Sync/GitHub/transboundary_fisheries_status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{071CA8C6-A7C6-4825-8DE5-4D9C653DB2FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEF7BEA-CAFC-AC42-B5AF-DAE80A45C031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{686FEDDD-4F38-4231-842C-27EB5C77BC16}"/>
+    <workbookView xWindow="10220" yWindow="2860" windowWidth="38640" windowHeight="21840" xr2:uid="{686FEDDD-4F38-4231-842C-27EB5C77BC16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
   <si>
     <t>stock_cs_id</t>
   </si>
@@ -342,6 +342,72 @@
   </si>
   <si>
     <t>total catch in this year from the RAM database</t>
+  </si>
+  <si>
+    <t>encoded unique identifier, joining stock ID and management program name</t>
+  </si>
+  <si>
+    <t>encoded RAM region containing the majority of the spatial distribution of the stock</t>
+  </si>
+  <si>
+    <t>encoded International Standard Statistical Classification of Aquatic Animals and Plants classification</t>
+  </si>
+  <si>
+    <t>encoded FAO region containing the majority of the spatial distribution of the stock</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 0% threshold</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 5% threshold</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 10% threshold</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 15% threshold</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 20% threshold</t>
+  </si>
+  <si>
+    <t>number of containing EEZs for this stock - 1, at a 25% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 0% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 0% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 5% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 5% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 10% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 10% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 15% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 15% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 20% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 20% threshold</t>
+  </si>
+  <si>
+    <t>binary indicator of whether or not a stock crosses two or more jurisdictions, at a 25% threshold</t>
+  </si>
+  <si>
+    <t>counter of total stocks shared, at a 25% threshold</t>
   </si>
 </sst>
 </file>
@@ -695,17 +761,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB96E6-C9AA-474E-A32F-DA5655CD31DE}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -713,7 +779,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -721,7 +787,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -729,7 +795,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -737,7 +803,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -745,7 +811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -753,7 +819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -761,7 +827,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -769,7 +835,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -777,7 +843,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -785,7 +851,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -793,7 +859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -801,7 +867,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -809,7 +875,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -817,7 +883,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -825,7 +891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -833,7 +899,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -841,7 +907,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -849,7 +915,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -857,7 +923,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -865,7 +931,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -873,7 +939,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -881,7 +947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -889,7 +955,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -897,7 +963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -905,7 +971,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -913,7 +979,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -921,7 +987,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -929,7 +995,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -937,7 +1003,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -945,7 +1011,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -953,7 +1019,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -961,7 +1027,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -969,7 +1035,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -977,7 +1043,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -985,7 +1051,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -993,7 +1059,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1001,7 +1067,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1009,7 +1075,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1017,7 +1083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1025,7 +1091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1033,114 +1099,180 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>